<commit_message>
fixing parameters so that ligand accumulates in some cases
</commit_message>
<xml_diff>
--- a/parameters/ModelG_Bevacizumab_VEGFR1_Params.xlsx
+++ b/parameters/ModelG_Bevacizumab_VEGFR1_Params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steinanf/git/TMDD_EndogenousLigand/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE56C65-C863-B54D-ADAB-E9563DB6926C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A670AE73-B0F5-1D4F-A303-AECADAE016E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -979,7 +979,7 @@
   <dimension ref="A1:J997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1629,7 +1629,7 @@
         <v>67</v>
       </c>
       <c r="I22" s="11" t="str">
-        <f t="shared" ref="I22:I31" ca="1" si="0">_xlfn.IFNA(_xlfn.FORMULATEXT(F22),"")</f>
+        <f t="shared" ref="I22:I29" ca="1" si="0">_xlfn.IFNA(_xlfn.FORMULATEXT(F22),"")</f>
         <v/>
       </c>
     </row>
@@ -1815,7 +1815,7 @@
         <v>80</v>
       </c>
       <c r="F28" s="14">
-        <v>8.7999999999999995E-2</v>
+        <v>9.3299999999999998E-3</v>
       </c>
       <c r="G28" t="s">
         <v>61</v>
@@ -1849,7 +1849,7 @@
       </c>
       <c r="F29" s="14">
         <f>(koff_TL+keTL)/kon_TL</f>
-        <v>9.3384502923976626E-2</v>
+        <v>1.0962301587301591</v>
       </c>
       <c r="G29" s="24" t="s">
         <v>61</v>
@@ -1880,8 +1880,8 @@
         <v>82</v>
       </c>
       <c r="F30" s="14">
-        <f>0.00135*3600*24</f>
-        <v>116.64000000000001</v>
+        <f>0.003*3600*24</f>
+        <v>259.20000000000005</v>
       </c>
       <c r="G30" t="s">
         <v>18</v>
@@ -1911,8 +1911,8 @@
         <v>83</v>
       </c>
       <c r="F31" s="14">
-        <f>15200000*3600*24/1000000000</f>
-        <v>1313.28</v>
+        <f>2800000*3600*24/1000000000</f>
+        <v>241.92</v>
       </c>
       <c r="G31" t="s">
         <v>70</v>

</xml_diff>